<commit_message>
Entregable 2 - Jose Carlos Diaz Faz
</commit_message>
<xml_diff>
--- a/exportaciones/resultados_matched.xlsx
+++ b/exportaciones/resultados_matched.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>score (%)</t>
+          <t>match_query</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>nombre_completo</t>
         </is>
@@ -478,10 +483,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>AprilGonzalezuser8@example.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>April Gonzalez</t>
         </is>
@@ -505,10 +515,15 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>ColtonCollinsuser9@example.com</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>Colton Collins</t>
         </is>
@@ -532,10 +547,15 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>JosephYanguser10@example.com</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Joseph Yang</t>
         </is>
@@ -559,10 +579,15 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>MichelleLoganuser11@example.com</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
         <is>
           <t>Michelle Logan</t>
         </is>
@@ -586,10 +611,15 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>MaryPollarduser12@example.com</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>Mary Pollard</t>
         </is>
@@ -613,10 +643,15 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>GailHarrisuser13@example.com</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>Gail Harris</t>
         </is>
@@ -640,10 +675,15 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>LaurenFletcheruser14@example.com</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Lauren Fletcher</t>
         </is>
@@ -667,10 +707,15 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>AlanLiuuser15@example.com</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Alan Liu</t>
         </is>
@@ -694,10 +739,15 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>DouglasWilliamsuser16@example.com</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>Douglas Williams</t>
         </is>
@@ -721,10 +771,15 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>DanielSmithuser17@example.com</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>Daniel Smith</t>
         </is>

</xml_diff>